<commit_message>
Fixed AU-B data not showing
</commit_message>
<xml_diff>
--- a/Stock On Hand Live - Marlborough - Wineworks (Manhattan) (1).xlsx
+++ b/Stock On Hand Live - Marlborough - Wineworks (Manhattan) (1).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A232DD-C7E9-450A-82EA-A367CACA6B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8844FAB7-F3D2-434A-8011-9633D4867B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32115" yWindow="3225" windowWidth="21600" windowHeight="11385" xr2:uid="{193EA25E-AA3D-4200-BC3D-0D30FA5D77C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19400" xr2:uid="{193EA25E-AA3D-4200-BC3D-0D30FA5D77C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2029,26 +2029,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7997337-1C16-413B-9F89-9E000A5F3DCF}">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E32" zoomScale="278" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.5" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>14</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>14</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>14</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>14</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>14</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>14</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>14</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
         <v>14</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
         <v>14</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
         <v>14</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>14</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>14</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
         <v>14</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
         <v>14</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
         <v>14</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
         <v>14</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
         <v>14</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A68" s="2" t="s">
         <v>14</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
         <v>14</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
         <v>14</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A71" s="2" t="s">
         <v>14</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
         <v>14</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A73" s="2" t="s">
         <v>14</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A74" s="2" t="s">
         <v>14</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A75" s="2" t="s">
         <v>14</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
         <v>14</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
         <v>14</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
         <v>14</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
         <v>14</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A80" s="2" t="s">
         <v>14</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A81" s="2" t="s">
         <v>14</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" s="2" t="s">
         <v>14</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" s="2" t="s">
         <v>14</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">
         <v>271</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
         <v>271</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A86" s="2" t="s">
         <v>271</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
         <v>271</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A88" s="2" t="s">
         <v>271</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A89" s="2" t="s">
         <v>271</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" s="2" t="s">
         <v>271</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A91" s="2" t="s">
         <v>271</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A92" s="2" t="s">
         <v>271</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A93" s="2" t="s">
         <v>271</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A94" s="2" t="s">
         <v>271</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
         <v>271</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A96" s="2" t="s">
         <v>271</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A97" s="2" t="s">
         <v>271</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
         <v>271</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
         <v>271</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
         <v>271</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
         <v>271</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
         <v>271</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
         <v>271</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
         <v>271</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
         <v>271</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
         <v>271</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
         <v>271</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
         <v>271</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
         <v>271</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="26" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
         <v>271</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
         <v>271</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A112" s="2" t="s">
         <v>271</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" ht="26" x14ac:dyDescent="0.15">
       <c r="A113" s="2" t="s">
         <v>271</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" ht="26" x14ac:dyDescent="0.15">
       <c r="A114" s="2" t="s">
         <v>271</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A115" s="2" t="s">
         <v>271</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A116" s="2" t="s">
         <v>271</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A117" s="2" t="s">
         <v>271</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A118" s="2" t="s">
         <v>271</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A119" s="2" t="s">
         <v>271</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A120" s="2" t="s">
         <v>271</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A121" s="2" t="s">
         <v>271</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A122" s="2" t="s">
         <v>271</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A123" s="2" t="s">
         <v>271</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A124" s="2" t="s">
         <v>271</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A125" s="2" t="s">
         <v>271</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A126" s="2" t="s">
         <v>271</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A127" s="2" t="s">
         <v>271</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A128" s="2" t="s">
         <v>271</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A129" s="2" t="s">
         <v>271</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A130" s="2" t="s">
         <v>271</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A131" s="2" t="s">
         <v>271</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A132" s="2" t="s">
         <v>271</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A133" s="2" t="s">
         <v>271</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A134" s="2" t="s">
         <v>271</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A135" s="2" t="s">
         <v>271</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A136" s="2" t="s">
         <v>271</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A137" s="2" t="s">
         <v>271</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A138" s="2" t="s">
         <v>271</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A139" s="2" t="s">
         <v>271</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
         <v>271</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
         <v>271</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
         <v>271</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
         <v>271</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
         <v>271</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
         <v>271</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
         <v>271</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
         <v>271</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
         <v>271</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A149" s="2" t="s">
         <v>271</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A150" s="2" t="s">
         <v>271</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A151" s="2" t="s">
         <v>271</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A152" s="2" t="s">
         <v>271</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A153" s="2" t="s">
         <v>271</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A154" s="2" t="s">
         <v>271</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A155" s="2" t="s">
         <v>271</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A156" s="2" t="s">
         <v>271</v>
       </c>
@@ -7630,16 +7630,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3144DCB1-9E52-4411-AF1F-194D24DD917A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="152.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="152.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="52" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -7647,7 +7649,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -7655,7 +7657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -7663,7 +7665,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -7671,7 +7673,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.8858267716535434" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -7683,21 +7685,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB49A99D5E78604598BEC347C9A30D03" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="19201c1866d1168e7c1bc741e77954a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4355520-101b-4542-a445-96baac0b68df" xmlns:ns3="247a2ce8-409f-4977-8c0a-1de402b244ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3c36ee63f48581d2a1eab2c464682f8" ns2:_="" ns3:_="">
     <xsd:import namespace="a4355520-101b-4542-a445-96baac0b68df"/>
@@ -7874,24 +7861,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E94EDD5-BC1F-425D-BF0A-73E875A79297}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E9826FD-8CA9-4D5B-852F-83EE8E8EC5B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B2E127-09AA-4B37-97E1-284311340360}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7908,4 +7893,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E9826FD-8CA9-4D5B-852F-83EE8E8EC5B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E94EDD5-BC1F-425D-BF0A-73E875A79297}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>